<commit_message>
Refactor AltitudeVelocity class: simplify AoC calculations and add time to climb method; update design parameters in JSON files for accuracy
</commit_message>
<xml_diff>
--- a/concepts.xlsx
+++ b/concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 1 Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 2 Data" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 3 Data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 4 Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Design 1 Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Design 2 Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Design 3 Data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Design 4 Data" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09022827764550193</v>
+        <v>0.09160635875461277</v>
       </c>
     </row>
     <row r="9">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>28682698.14258448</v>
+        <v>28251209.70656328</v>
       </c>
     </row>
     <row r="12">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.0905172449519278</v>
+        <v>0.09189973953757311</v>
       </c>
     </row>
     <row r="9">
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>28396564.09358083</v>
+        <v>27969380.11778452</v>
       </c>
     </row>
     <row r="12">
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>4704000</v>
+        <v>3704000</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -3196,7 +3196,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2660727.321062625</v>
+        <v>2576820.376306887</v>
       </c>
     </row>
     <row r="3">
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1300965.803637788</v>
+        <v>1271333.801151386</v>
       </c>
     </row>
     <row r="4">
@@ -3268,7 +3268,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1300540.803637788</v>
+        <v>1270908.801151386</v>
       </c>
     </row>
     <row r="5">
@@ -3304,7 +3304,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2190695.78095885</v>
+        <v>2160979.871527693</v>
       </c>
     </row>
     <row r="6">
@@ -3338,7 +3338,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.1532238838858399</v>
+        <v>0.1556965958011061</v>
       </c>
     </row>
     <row r="7">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.666673257969465</v>
+        <v>1.659202215491003</v>
       </c>
     </row>
     <row r="8">
@@ -3406,7 +3406,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09462125079283183</v>
+        <v>0.09532577852625242</v>
       </c>
     </row>
     <row r="9">
@@ -3505,7 +3505,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>28119764.83895933</v>
+        <v>27031726.52922251</v>
       </c>
     </row>
     <row r="12">
@@ -3523,7 +3523,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01840271129936119</v>
+        <v>0.01875923834870008</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3567,7 +3567,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>271226.0266118884</v>
+        <v>262672.8212341373</v>
       </c>
     </row>
     <row r="14">
@@ -3593,7 +3593,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>14.96656202861249</v>
+        <v>14.82365694186935</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -3601,7 +3601,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>532.423333135427</v>
+        <v>515.6461491277062</v>
       </c>
     </row>
     <row r="15">
@@ -3635,7 +3635,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>65.26397677956359</v>
+        <v>64.22748004570667</v>
       </c>
     </row>
     <row r="16">
@@ -3669,7 +3669,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>8.157997097445449</v>
+        <v>8.028435005713336</v>
       </c>
     </row>
     <row r="17">
@@ -3695,7 +3695,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.06710844165758807</v>
+        <v>0.07492631916093592</v>
       </c>
     </row>
     <row r="18">
@@ -3731,7 +3731,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1300965.803637788</v>
+        <v>1271333.801151386</v>
       </c>
     </row>
     <row r="19">
@@ -3757,7 +3757,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>107.5609874006116</v>
+        <v>102.1435295995264</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>470031.5401037745</v>
+        <v>415840.5047791936</v>
       </c>
     </row>
     <row r="20">
@@ -3791,7 +3791,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>38.56875491201791</v>
+        <v>38.70985876223332</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3799,7 +3799,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>517034.6941141519</v>
+        <v>457424.555257113</v>
       </c>
     </row>
     <row r="21">
@@ -3833,7 +3833,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>466085.9613534763</v>
+        <v>411893.1848250543</v>
       </c>
     </row>
     <row r="22">
@@ -3859,7 +3859,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>22.00055552259425</v>
+        <v>21.43935360960934</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -3867,7 +3867,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>3945.578750298126</v>
+        <v>3947.319954139297</v>
       </c>
     </row>
     <row r="23">
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>7.521557443621964</v>
+        <v>7.329693541746782</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -3893,7 +3893,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8233447161672861</v>
+        <v>0.830696946984754</v>
       </c>
     </row>
     <row r="24">
@@ -3921,7 +3921,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>2.256467233086589</v>
+        <v>2.198908062524035</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -3929,7 +3929,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2660727.321062625</v>
+        <v>2576820.376306887</v>
       </c>
     </row>
     <row r="25">
@@ -3963,7 +3963,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>24.94436869682966</v>
+        <v>24.5954683821708</v>
       </c>
     </row>
     <row r="26">
@@ -4041,7 +4041,7 @@
         </is>
       </c>
       <c r="H28" s="2" t="n">
-        <v>5.361520434171553</v>
+        <v>5.224755909245141</v>
       </c>
     </row>
     <row r="29">
@@ -4113,7 +4113,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>67.25661364414393</v>
+        <v>67.44847754601911</v>
       </c>
     </row>
     <row r="33">
@@ -4133,7 +4133,7 @@
         </is>
       </c>
       <c r="H33" s="2" t="n">
-        <v>0.9367482714051187</v>
+        <v>0.9382598023610346</v>
       </c>
     </row>
     <row r="34">
@@ -4181,7 +4181,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>83.26673013849133</v>
+        <v>78.81009788949248</v>
       </c>
     </row>
     <row r="37">
@@ -4199,7 +4199,7 @@
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>34.99856284603381</v>
+        <v>35.24373303523933</v>
       </c>
     </row>
     <row r="38">
@@ -4209,7 +4209,7 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>11.65428156777921</v>
+        <v>11.46919286530477</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4227,7 +4227,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>4.661712627111686</v>
+        <v>4.587677146121907</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -4235,7 +4235,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>11.17587111628158</v>
+        <v>10.87267891709485</v>
       </c>
     </row>
     <row r="40">
@@ -4245,7 +4245,7 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>13.98513788133506</v>
+        <v>13.76303143836572</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>11.55128797548484</v>
+        <v>11.23791102542103</v>
       </c>
     </row>
     <row r="41">
@@ -4263,7 +4263,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>29.3386711305069</v>
+        <v>29.34967068768253</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4271,7 +4271,7 @@
         </is>
       </c>
       <c r="H41" s="2" t="n">
-        <v>3.349873512890604</v>
+        <v>3.258994197372098</v>
       </c>
     </row>
     <row r="42">
@@ -4281,7 +4281,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>28.58946731543538</v>
+        <v>28.6123654320558</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4299,7 +4299,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>8.657466307493131</v>
+        <v>8.519971842797826</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4317,7 +4317,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>532.423333135427</v>
+        <v>515.6461491277062</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4325,7 +4325,7 @@
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>8.202906877061356</v>
+        <v>7.980368754538002</v>
       </c>
     </row>
     <row r="45">
@@ -4335,7 +4335,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>65.26397677956359</v>
+        <v>64.22748004570667</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -4361,7 +4361,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>63.22688311228104</v>
+        <v>63.54026006234486</v>
       </c>
     </row>
     <row r="47">
@@ -4371,7 +4371,7 @@
         </is>
       </c>
       <c r="H47" s="2" t="n">
-        <v>0.8891952741189892</v>
+        <v>0.8920929115484495</v>
       </c>
     </row>
     <row r="49">
@@ -4393,7 +4393,7 @@
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>31.76059207470455</v>
+        <v>31.73297120420188</v>
       </c>
     </row>
     <row r="51">

</xml_diff>

<commit_message>
Repository restructuring: added relevant files to class I folder.
</commit_message>
<xml_diff>
--- a/concepts.xlsx
+++ b/concepts.xlsx
@@ -438,7 +438,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2588931.195838803</v>
+        <v>2588964.198201469</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1275610.7753104</v>
+        <v>1275622.430198984</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1275185.7753104</v>
+        <v>1275197.430198984</v>
       </c>
     </row>
     <row r="5">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2165268.956506239</v>
+        <v>2165280.644397186</v>
       </c>
     </row>
     <row r="6">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.07196333532596165</v>
+        <v>0.07196287856928146</v>
       </c>
     </row>
     <row r="7">
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.651576516801808</v>
+        <v>1.651605656346414</v>
       </c>
     </row>
     <row r="8">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>14.37172940383783</v>
+        <v>14.37070569252619</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09131919534790821</v>
+        <v>0.09131141048528836</v>
       </c>
     </row>
     <row r="9">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>28350350.50380683</v>
+        <v>28353128.97306071</v>
       </c>
     </row>
     <row r="12">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01841095455040222</v>
+        <v>0.01841357768863145</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>263907.3594127221</v>
+        <v>263910.7235679377</v>
       </c>
     </row>
     <row r="14">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>514.9275934396583</v>
+        <v>514.9341300699099</v>
       </c>
     </row>
     <row r="15">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>55.58386061293287</v>
+        <v>55.58421341009927</v>
       </c>
     </row>
     <row r="16">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>9.263976768822145</v>
+        <v>9.264035568349879</v>
       </c>
     </row>
     <row r="17">
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.07632167846543067</v>
+        <v>0.07632548095692555</v>
       </c>
     </row>
     <row r="18">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>119.4319792272197</v>
+        <v>119.6033070112643</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1275610.7753104</v>
+        <v>1275622.430198984</v>
       </c>
     </row>
     <row r="19">
@@ -1081,7 +1081,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>38.14808712767177</v>
+        <v>38.09416660875394</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>423662.2393325642</v>
+        <v>423683.5538042828</v>
       </c>
     </row>
     <row r="20">
@@ -1123,7 +1123,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>466028.4632658207</v>
+        <v>466051.9091847111</v>
       </c>
     </row>
     <row r="21">
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>23.18283646412769</v>
+        <v>23.19945864779369</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>419563.9071338483</v>
+        <v>419584.810607416</v>
       </c>
     </row>
     <row r="22">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>7.925756056112032</v>
+        <v>7.931438853946561</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1191,7 +1191,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>4098.332198715885</v>
+        <v>4098.743196866766</v>
       </c>
     </row>
     <row r="23">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>2.37772681683361</v>
+        <v>2.379431656183968</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8206810696241504</v>
+        <v>0.8206740338348483</v>
       </c>
     </row>
     <row r="24">
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>23.7369947472405</v>
+        <v>23.73474478423399</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>2588931.195838803</v>
+        <v>2588964.198201469</v>
       </c>
     </row>
     <row r="26">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="H27" s="2" t="n">
-        <v>5.649641496408063</v>
+        <v>5.653692311274727</v>
       </c>
     </row>
     <row r="28">
@@ -1409,7 +1409,7 @@
         </is>
       </c>
       <c r="H30" s="2" t="n">
-        <v>18.68146222574916</v>
+        <v>18.68882058728235</v>
       </c>
     </row>
     <row r="31">
@@ -1427,7 +1427,7 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>66.90419934527672</v>
+        <v>66.89841397345116</v>
       </c>
     </row>
     <row r="32">
@@ -1445,7 +1445,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>0.9342536761800772</v>
+        <v>0.9342075400657516</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>64.66507002733304</v>
+        <v>64.76173353994677</v>
       </c>
     </row>
     <row r="36">
@@ -1503,7 +1503,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>37.1207061000251</v>
+        <v>37.06600542627907</v>
       </c>
     </row>
     <row r="37">
@@ -1541,7 +1541,7 @@
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>9.848736215423761</v>
+        <v>9.856094576956949</v>
       </c>
     </row>
     <row r="39">
@@ -1559,7 +1559,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>7.724498992489226</v>
+        <v>7.730270256436822</v>
       </c>
     </row>
     <row r="40">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>5.407149294742458</v>
+        <v>5.411189179505775</v>
       </c>
     </row>
     <row r="41">
@@ -1605,7 +1605,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>13.23425252688878</v>
+        <v>13.23433652621411</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1623,7 +1623,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>5.293701010755512</v>
+        <v>5.293734610485646</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>6.633981487667217</v>
+        <v>6.638937984939859</v>
       </c>
     </row>
     <row r="44">
@@ -1641,7 +1641,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>11.9108272741999</v>
+        <v>11.9109028735927</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1667,7 +1667,7 @@
         </is>
       </c>
       <c r="H45" s="2" t="n">
-        <v>67.05367209527665</v>
+        <v>67.04790083132906</v>
       </c>
     </row>
     <row r="46">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>29.18049505837779</v>
+        <v>29.18048965842116</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1685,7 +1685,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>0.920650806235558</v>
+        <v>0.9205945069050846</v>
       </c>
     </row>
     <row r="47">
@@ -1695,7 +1695,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>9.831159019974521</v>
+        <v>9.831221419473341</v>
       </c>
     </row>
     <row r="48">
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>514.9275934396583</v>
+        <v>514.9341300699099</v>
       </c>
       <c r="G48" s="1" t="inlineStr">
         <is>
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>55.58386061293287</v>
+        <v>55.58421341009927</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -1733,7 +1733,7 @@
         </is>
       </c>
       <c r="H49" s="2" t="n">
-        <v>31.96626811107582</v>
+        <v>32.01664710221132</v>
       </c>
     </row>
     <row r="50">
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2571935.136938421</v>
+        <v>2572020.246254603</v>
       </c>
     </row>
     <row r="3">
@@ -1919,7 +1919,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1269608.563442702</v>
+        <v>1269638.620066455</v>
       </c>
     </row>
     <row r="4">
@@ -1955,7 +1955,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1269183.563442702</v>
+        <v>1269213.620066455</v>
       </c>
     </row>
     <row r="5">
@@ -1991,7 +1991,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2159249.748579641</v>
+        <v>2159279.890312709</v>
       </c>
     </row>
     <row r="6">
@@ -2025,7 +2025,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.1118316192730599</v>
+        <v>0.111829776455133</v>
       </c>
     </row>
     <row r="7">
@@ -2059,7 +2059,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.765081965863206</v>
+        <v>1.765175244692074</v>
       </c>
     </row>
     <row r="8">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09135057340270591</v>
+        <v>0.09132671779534859</v>
       </c>
     </row>
     <row r="9">
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>28154559.31076002</v>
+        <v>28162845.5324341</v>
       </c>
     </row>
     <row r="12">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.02028989287058652</v>
+        <v>0.02030005954817041</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2254,7 +2254,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>262174.8355696658</v>
+        <v>262183.5113409381</v>
       </c>
     </row>
     <row r="14">
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>14.14085204481156</v>
+        <v>14.13731058997421</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -2288,7 +2288,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>511.7416290519052</v>
+        <v>511.7584949430478</v>
       </c>
     </row>
     <row r="15">
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>71.53611878288514</v>
+        <v>71.53729761062043</v>
       </c>
     </row>
     <row r="16">
@@ -2356,7 +2356,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>7.153611878288514</v>
+        <v>7.153729761062041</v>
       </c>
     </row>
     <row r="17">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.07436348128584291</v>
+        <v>0.07437328679825092</v>
       </c>
     </row>
     <row r="18">
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1269608.563442702</v>
+        <v>1269638.620066455</v>
       </c>
     </row>
     <row r="19">
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>155.78342869607</v>
+        <v>156.2894430915086</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>412685.3883587799</v>
+        <v>412740.3559418936</v>
       </c>
     </row>
     <row r="20">
@@ -2478,7 +2478,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>22.44422613983506</v>
+        <v>22.37266501988687</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2486,7 +2486,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>453953.9271946579</v>
+        <v>454014.391536083</v>
       </c>
     </row>
     <row r="21">
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>408799.0906868614</v>
+        <v>408852.9946258218</v>
       </c>
     </row>
     <row r="22">
@@ -2546,7 +2546,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>26.4768848079285</v>
+        <v>26.51985094060275</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>3886.297671918524</v>
+        <v>3887.361316071823</v>
       </c>
     </row>
     <row r="23">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>9.051926430061025</v>
+        <v>9.066615706188974</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8296383408101521</v>
+        <v>0.8296150510912133</v>
       </c>
     </row>
     <row r="24">
@@ -2608,7 +2608,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>2.715577929018307</v>
+        <v>2.719984711856692</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2616,7 +2616,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2571935.136938422</v>
+        <v>2572020.246254603</v>
       </c>
     </row>
     <row r="25">
@@ -2650,7 +2650,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>24.96132936763262</v>
+        <v>24.95485372195421</v>
       </c>
     </row>
     <row r="26">
@@ -2728,7 +2728,7 @@
         </is>
       </c>
       <c r="H28" s="2" t="n">
-        <v>6.452398839889653</v>
+        <v>6.46286965723214</v>
       </c>
     </row>
     <row r="29">
@@ -2790,7 +2790,7 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>13.45259935749131</v>
+        <v>13.46478894403764</v>
       </c>
     </row>
     <row r="32">
@@ -2808,7 +2808,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>42.25105932373255</v>
+        <v>42.2340451262468</v>
       </c>
     </row>
     <row r="33">
@@ -2826,7 +2826,7 @@
         </is>
       </c>
       <c r="H33" s="2" t="n">
-        <v>0.8407018734645043</v>
+        <v>0.840443527069524</v>
       </c>
     </row>
     <row r="34">
@@ -2868,7 +2868,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>70.04070144610718</v>
+        <v>70.27649321185062</v>
       </c>
     </row>
     <row r="37">
@@ -2886,7 +2886,7 @@
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>21.91728457949396</v>
+        <v>21.84482757518156</v>
       </c>
     </row>
     <row r="38">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>7.247794566941063</v>
+        <v>7.259984153487387</v>
       </c>
     </row>
     <row r="40">
@@ -2940,7 +2940,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>11.36908951677029</v>
+        <v>11.38821043684296</v>
       </c>
     </row>
     <row r="41">
@@ -2950,7 +2950,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>10.21944554041216</v>
+        <v>10.21961394437434</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2958,7 +2958,7 @@
         </is>
       </c>
       <c r="H41" s="2" t="n">
-        <v>7.958362661739205</v>
+        <v>7.971747305790071</v>
       </c>
     </row>
     <row r="42">
@@ -2968,7 +2968,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>4.087778216164866</v>
+        <v>4.087845577749738</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>15.32916831061825</v>
+        <v>15.32942091656152</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>20.48900923861207</v>
+        <v>20.48899923060518</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>9.764041584990958</v>
+        <v>9.780463081053366</v>
       </c>
     </row>
     <row r="45">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>19.83204488244272</v>
+        <v>19.83202404846683</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -3040,7 +3040,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>7.59158811573475</v>
+        <v>7.591713215820942</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -3048,7 +3048,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>41.07175120290683</v>
+        <v>41.05263028283417</v>
       </c>
     </row>
     <row r="47">
@@ -3058,7 +3058,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>511.7416290519052</v>
+        <v>511.7584949430478</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -3066,7 +3066,7 @@
         </is>
       </c>
       <c r="H47" s="2" t="n">
-        <v>0.830731224331671</v>
+        <v>0.8304561089610522</v>
       </c>
     </row>
     <row r="48">
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>71.53611878288514</v>
+        <v>71.53729761062043</v>
       </c>
     </row>
     <row r="49">
@@ -3106,7 +3106,7 @@
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>21.878441149811</v>
+        <v>21.93620008524906</v>
       </c>
     </row>
     <row r="51">
@@ -3128,7 +3128,7 @@
         </is>
       </c>
       <c r="H52" s="2" t="n">
-        <v>20.36283114795463</v>
+        <v>20.3628356137201</v>
       </c>
     </row>
     <row r="53">
@@ -3248,7 +3248,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2576599.359620654</v>
+        <v>2576612.94395303</v>
       </c>
     </row>
     <row r="3">
@@ -3284,7 +3284,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1271255.748410757</v>
+        <v>1271260.54576063</v>
       </c>
     </row>
     <row r="4">
@@ -3320,7 +3320,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1270830.748410757</v>
+        <v>1270835.54576063</v>
       </c>
     </row>
     <row r="5">
@@ -3356,7 +3356,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2160901.597770378</v>
+        <v>2160906.408704584</v>
       </c>
     </row>
     <row r="6">
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.1557032689944218</v>
+        <v>0.1557028617907942</v>
       </c>
     </row>
     <row r="7">
@@ -3424,7 +3424,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.659182757136198</v>
+        <v>1.659216450185598</v>
       </c>
     </row>
     <row r="8">
@@ -3458,7 +3458,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09537792017760385</v>
+        <v>0.09537320004849245</v>
       </c>
     </row>
     <row r="9">
@@ -3557,7 +3557,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>27014631.42436689</v>
+        <v>27016110.84290925</v>
       </c>
     </row>
     <row r="12">
@@ -3575,7 +3575,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01873392195678794</v>
+        <v>0.01873621119097947</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3619,7 +3619,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>262650.2915005764</v>
+        <v>262651.6762439378</v>
       </c>
     </row>
     <row r="14">
@@ -3645,7 +3645,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>14.83366965595746</v>
+        <v>14.83276342201457</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>515.6019505348337</v>
+        <v>515.6046474057424</v>
       </c>
     </row>
     <row r="15">
@@ -3687,7 +3687,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>64.22472735853901</v>
+        <v>64.22489532296599</v>
       </c>
     </row>
     <row r="16">
@@ -3721,7 +3721,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>8.028090919817377</v>
+        <v>8.028111915370749</v>
       </c>
     </row>
     <row r="17">
@@ -3747,7 +3747,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.07490085515794141</v>
+        <v>0.07490242024942624</v>
       </c>
     </row>
     <row r="18">
@@ -3783,7 +3783,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1271255.748410757</v>
+        <v>1271260.54576063</v>
       </c>
     </row>
     <row r="19">
@@ -3809,7 +3809,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>102.1294162888502</v>
+        <v>102.2506970670776</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -3817,7 +3817,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>415697.761850276</v>
+        <v>415706.535248447</v>
       </c>
     </row>
     <row r="20">
@@ -3843,7 +3843,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>38.71023049276001</v>
+        <v>38.66461917669569</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3851,7 +3851,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>457267.5380353036</v>
+        <v>457277.1887732917</v>
       </c>
     </row>
     <row r="21">
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>411753.2013131287</v>
+        <v>411761.8051058073</v>
       </c>
     </row>
     <row r="22">
@@ -3911,7 +3911,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>21.43787240609072</v>
+        <v>21.45059758612448</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -3919,7 +3919,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>3944.560537147278</v>
+        <v>3944.730142639659</v>
       </c>
     </row>
     <row r="23">
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>7.329187147381443</v>
+        <v>7.333537636281872</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -3945,7 +3945,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8307710532707838</v>
+        <v>0.8307664987870182</v>
       </c>
     </row>
     <row r="24">
@@ -3973,7 +3973,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>2.198756144214433</v>
+        <v>2.200061290884562</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -3981,7 +3981,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2576599.359620654</v>
+        <v>2576612.94395303</v>
       </c>
     </row>
     <row r="25">
@@ -4015,7 +4015,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>24.61176775658028</v>
+        <v>24.61076526887319</v>
       </c>
     </row>
     <row r="26">
@@ -4093,7 +4093,7 @@
         </is>
       </c>
       <c r="H28" s="2" t="n">
-        <v>5.224394940953951</v>
+        <v>5.227496058682975</v>
       </c>
     </row>
     <row r="29">
@@ -4173,7 +4173,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>67.44898394038444</v>
+        <v>67.44463345148401</v>
       </c>
     </row>
     <row r="33">
@@ -4191,7 +4191,7 @@
         </is>
       </c>
       <c r="H33" s="2" t="n">
-        <v>0.9382637918074683</v>
+        <v>0.9382295180405841</v>
       </c>
     </row>
     <row r="34">
@@ -4233,7 +4233,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>76.33663273247861</v>
+        <v>76.43684226252361</v>
       </c>
     </row>
     <row r="37">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>36.38102495197497</v>
+        <v>36.33361409745591</v>
       </c>
     </row>
     <row r="38">
@@ -4287,7 +4287,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>10.70069853321352</v>
+        <v>10.70771980366434</v>
       </c>
     </row>
     <row r="40">
@@ -4305,7 +4305,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>8.91724877767793</v>
+        <v>8.923099836386946</v>
       </c>
     </row>
     <row r="41">
@@ -4315,7 +4315,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>11.46870131402482</v>
+        <v>11.4687313076725</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4323,7 +4323,7 @@
         </is>
       </c>
       <c r="H41" s="2" t="n">
-        <v>5.350349266606758</v>
+        <v>5.353859901832167</v>
       </c>
     </row>
     <row r="42">
@@ -4333,7 +4333,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>4.587480525609929</v>
+        <v>4.587492523069</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4351,7 +4351,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>13.76244157682979</v>
+        <v>13.762477569207</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4369,7 +4369,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>29.34969989987288</v>
+        <v>29.34969811739325</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4377,7 +4377,7 @@
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>7.282419835103642</v>
+        <v>7.287198199716006</v>
       </c>
     </row>
     <row r="45">
@@ -4387,7 +4387,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>28.61242624397128</v>
+        <v>28.61242253332858</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>8.51960669041844</v>
+        <v>8.519628971413857</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -4413,7 +4413,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>65.86092231008796</v>
+        <v>65.85507125137894</v>
       </c>
     </row>
     <row r="47">
@@ -4423,7 +4423,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>515.6019505348337</v>
+        <v>515.6046474057424</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="H47" s="2" t="n">
-        <v>0.9072400533887215</v>
+        <v>0.9071818107580653</v>
       </c>
     </row>
     <row r="48">
@@ -4441,7 +4441,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>64.22472735853901</v>
+        <v>64.22489532296599</v>
       </c>
     </row>
     <row r="49">
@@ -4471,7 +4471,7 @@
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>31.73289899401704</v>
+        <v>31.77593709834741</v>
       </c>
     </row>
     <row r="51">
@@ -5264,7 +5264,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>32.14959439464186</v>
+        <v>32.22366166980459</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Enhance fuel calculations and update design data
- Added conversions for fuel quantities from Newtons to liters in ClassIWeightEstimation.py.
- Updated AircraftIteration class to include maximum fuel in liters for design, ferry, altitude, and max outputs.
- Modified design JSON files (design1.json, design2.json, design3.json, design4.json) to include new fuel metrics in liters.
- Adjusted utils.py to reflect new fuel metrics in the design JSON to Excel conversion function.
- Updated concepts.xlsx to include changes related to fuel metrics.
</commit_message>
<xml_diff>
--- a/concepts.xlsx
+++ b/concepts.xlsx
@@ -438,7 +438,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2618138.067285629</v>
+        <v>2617230.057129697</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1285925.274185932</v>
+        <v>1285604.607532217</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1285500.274185932</v>
+        <v>1285179.607532217</v>
       </c>
     </row>
     <row r="5">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2175612.662253217</v>
+        <v>2175291.087589347</v>
       </c>
     </row>
     <row r="6">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.07839148154855212</v>
+        <v>0.07818974950738743</v>
       </c>
     </row>
     <row r="7">
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.613479079304364</v>
+        <v>1.614820666231021</v>
       </c>
     </row>
     <row r="8">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>13.58135197190163</v>
+        <v>13.6023089546819</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.08455401129295033</v>
+        <v>0.08478783657025808</v>
       </c>
     </row>
     <row r="9">
@@ -756,7 +756,7 @@
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>4850602117.146465</v>
+        <v>4837280592.753655</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.00126964877111443</v>
+        <v>0.001270043469758956</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="K10" s="2" t="n">
-        <v>5027.539614379501</v>
+        <v>4999.962615982123</v>
       </c>
     </row>
     <row r="11">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>30964090.61203126</v>
+        <v>30867989.59613708</v>
       </c>
     </row>
     <row r="12">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01809642563585512</v>
+        <v>0.0180407065178009</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="H12" s="2" t="n">
-        <v>46574052.27844714</v>
+        <v>46205736.73514064</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -887,11 +887,11 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>total_fuel_L [L]</t>
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>266884.6144022048</v>
+        <v>54938.8341339537</v>
       </c>
     </row>
     <row r="14">
@@ -917,15 +917,15 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>64.995</v>
+        <v>64.8165</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>mission_fuel_L [L]</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>520.7295620871082</v>
+        <v>54385.67286980832</v>
       </c>
     </row>
     <row r="15">
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>61.9</v>
+        <v>61.73</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -955,11 +955,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>reserve_fuel_L [L]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>51.02595232267146</v>
+        <v>553.1612641453846</v>
       </c>
     </row>
     <row r="16">
@@ -969,7 +969,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>61.9</v>
+        <v>61.73</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -981,11 +981,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>max_fuel_L [L]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>10.20519046453429</v>
+        <v>60432.71754734909</v>
       </c>
     </row>
     <row r="17">
@@ -1017,11 +1017,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.07968705477213764</v>
+        <v>266792.0547532821</v>
       </c>
     </row>
     <row r="18">
@@ -1047,15 +1047,15 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>132.9877637924719</v>
+        <v>134.0936683963558</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1285925.274185932</v>
+        <v>523.4200260289563</v>
       </c>
     </row>
     <row r="19">
@@ -1081,15 +1081,15 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>38.16554230424591</v>
+        <v>38.14450654420889</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>442525.4050324112</v>
+        <v>51.15760090294287</v>
       </c>
     </row>
     <row r="20">
@@ -1119,11 +1119,11 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>max_fuel [N]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>486777.9455356524</v>
+        <v>10.23152018058857</v>
       </c>
     </row>
     <row r="21">
@@ -1149,15 +1149,15 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>24.46313424453464</v>
+        <v>24.56463937825266</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>mission_fuel [N]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>438064.4231157815</v>
+        <v>0.07958242297173541</v>
       </c>
     </row>
     <row r="22">
@@ -1183,15 +1183,15 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>8.363464698986203</v>
+        <v>8.398167308804327</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>4460.981916629768</v>
+        <v>1285604.607532217</v>
       </c>
     </row>
     <row r="23">
@@ -1209,15 +1209,15 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>2.509039409695861</v>
+        <v>2.519450192641298</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Mff</t>
+          <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8114696678305754</v>
+        <v>441938.9695403504</v>
       </c>
     </row>
     <row r="24">
@@ -1249,11 +1249,11 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>21.91322727564344</v>
+        <v>486132.8664943855</v>
       </c>
     </row>
     <row r="25">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>MTOW [N]</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>2618138.067285629</v>
+        <v>437489.2296993121</v>
       </c>
     </row>
     <row r="26">
@@ -1315,6 +1315,14 @@
       <c r="H26" s="2" t="n">
         <v>0.3</v>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>4449.739841038303</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1339,7 +1347,15 @@
         </is>
       </c>
       <c r="H27" s="2" t="n">
-        <v>5.961649195687601</v>
+        <v>5.986385927814366</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0.8117510033563166</v>
       </c>
     </row>
     <row r="28">
@@ -1367,6 +1383,14 @@
       <c r="H28" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>21.9652896084792</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1393,6 +1417,14 @@
       <c r="H29" s="2" t="n">
         <v>4.5</v>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>2617230.057129697</v>
+      </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
@@ -1409,7 +1441,15 @@
         </is>
       </c>
       <c r="H30" s="2" t="n">
-        <v>18.31490099298168</v>
+        <v>18.35485255942574</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>total_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>54938.8341339537</v>
       </c>
     </row>
     <row r="31">
@@ -1427,7 +1467,15 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>66.89793710157005</v>
+        <v>66.86495379374394</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>mission_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>54385.67286980832</v>
       </c>
     </row>
     <row r="32">
@@ -1445,7 +1493,15 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>0.9365519746349722</v>
+        <v>0.9363014827246962</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>reserve_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>553.1612641453846</v>
       </c>
     </row>
     <row r="33">
@@ -1457,6 +1513,14 @@
       <c r="E33" s="2" t="n">
         <v>1.5</v>
       </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>max_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>60432.71754734907</v>
+      </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
@@ -1493,7 +1557,7 @@
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>59.94109493447505</v>
+        <v>60.44726267805435</v>
       </c>
     </row>
     <row r="36">
@@ -1503,7 +1567,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>37.17661027568419</v>
+        <v>37.15138198133811</v>
       </c>
     </row>
     <row r="37">
@@ -1541,7 +1605,7 @@
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>9.482174982656279</v>
+        <v>9.522126549100339</v>
       </c>
     </row>
     <row r="39">
@@ -1559,7 +1623,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>7.43699998639708</v>
+        <v>7.468334548313991</v>
       </c>
     </row>
     <row r="40">
@@ -1577,7 +1641,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>5.205899990477955</v>
+        <v>5.227834183819794</v>
       </c>
     </row>
     <row r="41">
@@ -1605,7 +1669,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>14.57884352076328</v>
+        <v>14.61645740084082</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1623,7 +1687,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>5.83153740830531</v>
+        <v>5.846582960336328</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1631,7 +1695,7 @@
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>6.387070576552786</v>
+        <v>6.41398143561084</v>
       </c>
     </row>
     <row r="44">
@@ -1641,7 +1705,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>10.93413264057246</v>
+        <v>10.96234305063062</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1667,7 +1731,7 @@
         </is>
       </c>
       <c r="H45" s="2" t="n">
-        <v>67.3411711013688</v>
+        <v>67.30983653945189</v>
       </c>
     </row>
     <row r="46">
@@ -1677,7 +1741,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>29.09405706591443</v>
+        <v>29.09163903076659</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1685,7 +1749,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>0.923455391453239</v>
+        <v>0.9231497192690139</v>
       </c>
     </row>
     <row r="47">
@@ -1695,7 +1759,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>10.82999804399557</v>
+        <v>10.85793978348175</v>
       </c>
     </row>
     <row r="48">
@@ -1705,7 +1769,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>520.7295620871082</v>
+        <v>523.4200260289563</v>
       </c>
       <c r="G48" s="1" t="inlineStr">
         <is>
@@ -1725,7 +1789,7 @@
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>51.02595232267146</v>
+        <v>51.15760090294287</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -1733,7 +1797,7 @@
         </is>
       </c>
       <c r="H49" s="2" t="n">
-        <v>32.12335290213378</v>
+        <v>32.1253565723892</v>
       </c>
     </row>
     <row r="50">
@@ -2250,11 +2314,11 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>max_fuel_L [L]</t>
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>255365.0821417169</v>
+        <v>50532.6180386827</v>
       </c>
     </row>
     <row r="14">
@@ -2284,11 +2348,11 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>total_fuel_L [L]</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>498.4583613440194</v>
+        <v>45938.74367152973</v>
       </c>
     </row>
     <row r="15">
@@ -2318,11 +2382,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>mission_fuel_L [L]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>70.60158364682901</v>
+        <v>45560.14901022315</v>
       </c>
     </row>
     <row r="16">
@@ -2352,11 +2416,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>reserve_fuel_L [L]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>7.060158364682901</v>
+        <v>378.5946613065801</v>
       </c>
     </row>
     <row r="17">
@@ -2378,11 +2442,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.06666805535102044</v>
+        <v>255365.0821417169</v>
       </c>
     </row>
     <row r="18">
@@ -2414,11 +2478,11 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1246016.632511913</v>
+        <v>498.4583613440194</v>
       </c>
     </row>
     <row r="19">
@@ -2448,11 +2512,11 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>369540.4418425194</v>
+        <v>70.60158364682901</v>
       </c>
     </row>
     <row r="20">
@@ -2482,11 +2546,11 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>max_fuel [N]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>406494.4860267714</v>
+        <v>7.060158364682901</v>
       </c>
     </row>
     <row r="21">
@@ -2516,11 +2580,11 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>mission_fuel [N]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>366494.9506680371</v>
+        <v>0.06666805535102044</v>
       </c>
     </row>
     <row r="22">
@@ -2550,11 +2614,11 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>3045.491174482391</v>
+        <v>1246016.632511913</v>
       </c>
     </row>
     <row r="23">
@@ -2576,11 +2640,11 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Mff</t>
+          <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8524866066467567</v>
+        <v>369540.4418425194</v>
       </c>
     </row>
     <row r="24">
@@ -2612,11 +2676,11 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>MTOW [N]</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2505131.455810243</v>
+        <v>406494.4860267714</v>
       </c>
     </row>
     <row r="25">
@@ -2646,11 +2710,11 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>31.49782606412045</v>
+        <v>366494.9506680371</v>
       </c>
     </row>
     <row r="26">
@@ -2678,6 +2742,14 @@
       <c r="H26" s="2" t="n">
         <v>0.8058156302009339</v>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>3045.491174482391</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2704,6 +2776,14 @@
       <c r="H27" s="2" t="n">
         <v>6.045074574692466</v>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0.8524866066467567</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2730,6 +2810,14 @@
       <c r="H28" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>2505131.455810243</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2756,6 +2844,14 @@
       <c r="H29" s="2" t="n">
         <v>4.5</v>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>31.49782606412045</v>
+      </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
@@ -2774,6 +2870,14 @@
       <c r="H30" s="2" t="n">
         <v>13.56035060683296</v>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>total_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>45938.74367152973</v>
+      </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
@@ -2792,6 +2896,14 @@
       <c r="H31" s="2" t="n">
         <v>39.79747992235293</v>
       </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>mission_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>45560.14901022315</v>
+      </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
@@ -2810,6 +2922,14 @@
       <c r="H32" s="2" t="n">
         <v>0.8050784543581808</v>
       </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>reserve_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>378.5946613065801</v>
+      </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
@@ -2819,6 +2939,14 @@
       </c>
       <c r="E33" s="2" t="n">
         <v>8.5</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>max_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>50532.6180386827</v>
       </c>
     </row>
     <row r="34">
@@ -3238,7 +3366,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2538385.611296866</v>
+        <v>2538415.641737442</v>
       </c>
     </row>
     <row r="3">
@@ -3274,7 +3402,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1257760.442525868</v>
+        <v>1257771.047870782</v>
       </c>
     </row>
     <row r="4">
@@ -3310,7 +3438,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1257335.442525868</v>
+        <v>1257346.047870782</v>
       </c>
     </row>
     <row r="5">
@@ -3346,7 +3474,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2147368.078137165</v>
+        <v>2147378.71351252</v>
       </c>
     </row>
     <row r="6">
@@ -3380,7 +3508,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.1568701469484847</v>
+        <v>0.1568692251654692</v>
       </c>
     </row>
     <row r="7">
@@ -3414,7 +3542,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.655176016017555</v>
+        <v>1.655258149774672</v>
       </c>
     </row>
     <row r="8">
@@ -3448,7 +3576,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.1056333557645627</v>
+        <v>0.1056332659449669</v>
       </c>
     </row>
     <row r="9">
@@ -3547,7 +3675,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>24030152.15150847</v>
+        <v>24030456.87387829</v>
       </c>
     </row>
     <row r="12">
@@ -3565,7 +3693,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01888395984380869</v>
+        <v>0.01888976835334421</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3605,11 +3733,11 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>max_fuel_L [L]</t>
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>258754.9043116071</v>
+        <v>53472.14403513278</v>
       </c>
     </row>
     <row r="14">
@@ -3635,15 +3763,15 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.81716800768987</v>
+        <v>16.81458221126043</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>total_fuel_L [L]</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>507.9598733705383</v>
+        <v>48611.04003193889</v>
       </c>
     </row>
     <row r="15">
@@ -3673,11 +3801,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>mission_fuel_L [L]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>63.74699198365603</v>
+        <v>48180.18163096658</v>
       </c>
     </row>
     <row r="16">
@@ -3707,11 +3835,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>reserve_fuel_L [L]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>7.968373997957004</v>
+        <v>430.858400972309</v>
       </c>
     </row>
     <row r="17">
@@ -3733,11 +3861,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.07049848337276755</v>
+        <v>258757.9655185976</v>
       </c>
     </row>
     <row r="18">
@@ -3769,11 +3897,11 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1257760.442525868</v>
+        <v>507.9658430584618</v>
       </c>
     </row>
     <row r="19">
@@ -3799,15 +3927,15 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>97.59645382784237</v>
+        <v>97.89060565452871</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>391017.5331597011</v>
+        <v>63.7473665688842</v>
       </c>
     </row>
     <row r="20">
@@ -3833,15 +3961,15 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>39.61091285692487</v>
+        <v>39.49258206671682</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>max_fuel [N]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>430119.2864756712</v>
+        <v>7.968420821110524</v>
       </c>
     </row>
     <row r="21">
@@ -3867,15 +3995,15 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>20.95671830762848</v>
+        <v>20.98827590454679</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>mission_fuel [N]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>387551.9999771285</v>
+        <v>0.07050194271916771</v>
       </c>
     </row>
     <row r="22">
@@ -3901,15 +4029,15 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>7.164690019702045</v>
+        <v>7.175478941725396</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>3465.533182572573</v>
+        <v>1257771.047870782</v>
       </c>
     </row>
     <row r="23">
@@ -3927,15 +4055,15 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>2.149407005910613</v>
+        <v>2.152643682517619</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Mff</t>
+          <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8438132763101673</v>
+        <v>391036.9282249228</v>
       </c>
     </row>
     <row r="24">
@@ -3967,11 +4095,11 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>MTOW [N]</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2538385.611296866</v>
+        <v>430140.6210474151</v>
       </c>
     </row>
     <row r="25">
@@ -4001,11 +4129,11 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>27.83536996194485</v>
+        <v>387571.0170758213</v>
       </c>
     </row>
     <row r="26">
@@ -4033,6 +4161,14 @@
       <c r="H26" s="2" t="n">
         <v>0.3</v>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>3465.911149101448</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4057,7 +4193,15 @@
         </is>
       </c>
       <c r="H27" s="2" t="n">
-        <v>5.107138014044021</v>
+        <v>5.114828578973488</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0.8438028261990694</v>
       </c>
     </row>
     <row r="28">
@@ -4085,6 +4229,14 @@
       <c r="H28" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>2538415.641737442</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4101,7 +4253,7 @@
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -4111,6 +4263,14 @@
       <c r="H29" s="2" t="n">
         <v>4.5</v>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>27.83247462486353</v>
+      </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
@@ -4119,7 +4279,7 @@
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -4129,6 +4289,14 @@
       <c r="H30" s="2" t="n">
         <v>8.832726010325398</v>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>total_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>48611.04003193889</v>
+      </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
@@ -4145,7 +4313,15 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>67.61348106806383</v>
+        <v>67.60269214604048</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>mission_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>48180.18163096658</v>
       </c>
     </row>
     <row r="32">
@@ -4163,7 +4339,15 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>0.9506383275514577</v>
+        <v>0.9505700135728937</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>reserve_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>430.858400972309</v>
       </c>
     </row>
     <row r="33">
@@ -4175,6 +4359,14 @@
       <c r="E33" s="2" t="n">
         <v>8.5</v>
       </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>max_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>53472.14403513278</v>
+      </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
@@ -4203,7 +4395,7 @@
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>74.5425072102618</v>
+        <v>74.79953332310792</v>
       </c>
     </row>
     <row r="36">
@@ -4223,7 +4415,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>36.43142971762163</v>
+        <v>36.30688408377614</v>
       </c>
     </row>
     <row r="37">
@@ -4241,7 +4433,7 @@
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>10.57420260896266</v>
+        <v>10.59241709831434</v>
       </c>
     </row>
     <row r="38">
@@ -4259,7 +4451,7 @@
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>8.811835507468881</v>
+        <v>8.82701424859528</v>
       </c>
     </row>
     <row r="39">
@@ -4277,7 +4469,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>5.287101304481329</v>
+        <v>5.296208549157168</v>
       </c>
     </row>
     <row r="40">
@@ -4305,7 +4497,7 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>11.38339142565286</v>
+        <v>11.38345831587218</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4323,7 +4515,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>4.553356570261146</v>
+        <v>4.553383326348871</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4341,7 +4533,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>13.66006971078344</v>
+        <v>13.66014997904661</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4349,7 +4541,7 @@
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>65.966335580297</v>
+        <v>65.95115683917061</v>
       </c>
     </row>
     <row r="44">
@@ -4359,7 +4551,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>29.35476974466756</v>
+        <v>30.03126843510636</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4367,7 +4559,7 @@
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>0.9082893585603768</v>
+        <v>0.9081382662782423</v>
       </c>
     </row>
     <row r="45">
@@ -4377,7 +4569,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>28.62298029587559</v>
+        <v>29.29947468622886</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -4385,7 +4577,7 @@
         </is>
       </c>
       <c r="H45" s="2" t="n">
-        <v>7.196332331099585</v>
+        <v>7.208728303019477</v>
       </c>
     </row>
     <row r="46">
@@ -4395,7 +4587,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>8.456233630484984</v>
+        <v>8.456283320362189</v>
       </c>
     </row>
     <row r="47">
@@ -4405,7 +4597,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>507.9598733705383</v>
+        <v>507.9658430584618</v>
       </c>
       <c r="G47" s="1" t="inlineStr">
         <is>
@@ -4425,7 +4617,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>63.74699198365603</v>
+        <v>63.7473665688842</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -4433,7 +4625,7 @@
         </is>
       </c>
       <c r="H48" s="2" t="n">
-        <v>31.76127414157109</v>
+        <v>31.87447604320883</v>
       </c>
     </row>
     <row r="49">
@@ -4950,11 +5142,11 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>MTOM [kg]</t>
+          <t>max_fuel_L [L]</t>
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>263578.3926925393</v>
+        <v>57648.46529873692</v>
       </c>
     </row>
     <row r="14">
@@ -4984,11 +5176,11 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>S [m²]</t>
+          <t>total_fuel_L [L]</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>561.0633135905323</v>
+        <v>52407.69572612447</v>
       </c>
     </row>
     <row r="15">
@@ -5018,11 +5210,11 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>b [m]</t>
+          <t>mission_fuel_L [L]</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>41.02669790236105</v>
+        <v>51903.21685673379</v>
       </c>
     </row>
     <row r="16">
@@ -5044,11 +5236,11 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>MAC [m]</t>
+          <t>reserve_fuel_L [L]</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>13.67556596745369</v>
+        <v>504.4788693906718</v>
       </c>
     </row>
     <row r="17">
@@ -5080,11 +5272,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>fuel_economy [L/ton/km]</t>
+          <t>MTOM [kg]</t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.07594985111932576</v>
+        <v>263578.3926925393</v>
       </c>
     </row>
     <row r="18">
@@ -5106,11 +5298,11 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>OEW [N]</t>
+          <t>S [m²]</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1274471.092321406</v>
+        <v>561.0633135905323</v>
       </c>
     </row>
     <row r="19">
@@ -5142,11 +5334,11 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>total_fuel [N]</t>
+          <t>b [m]</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>421577.9859600904</v>
+        <v>41.02669790236105</v>
       </c>
     </row>
     <row r="20">
@@ -5168,11 +5360,11 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>max_fuel [N]</t>
+          <t>MAC [m]</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>463735.7845560995</v>
+        <v>13.67556596745369</v>
       </c>
     </row>
     <row r="21">
@@ -5204,11 +5396,11 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>mission_fuel [N]</t>
+          <t>fuel_economy [L/ton/km]</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>417519.857038938</v>
+        <v>0.07594985111932576</v>
       </c>
     </row>
     <row r="22">
@@ -5238,11 +5430,11 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>reserve_fuel [N]</t>
+          <t>OEW [N]</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>4058.128921152442</v>
+        <v>1274471.092321406</v>
       </c>
     </row>
     <row r="23">
@@ -5266,11 +5458,11 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Mff</t>
+          <t>total_fuel [N]</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.8239224430163152</v>
+        <v>421577.9859600904</v>
       </c>
     </row>
     <row r="24">
@@ -5302,11 +5494,11 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>MTOW [N]</t>
+          <t>max_fuel [N]</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>2585704.03231381</v>
+        <v>463735.7845560995</v>
       </c>
     </row>
     <row r="25">
@@ -5338,11 +5530,11 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>mission_fuel [N]</t>
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>23.95928996628532</v>
+        <v>417519.857038938</v>
       </c>
     </row>
     <row r="26">
@@ -5362,6 +5554,14 @@
       <c r="E26" s="2" t="n">
         <v>0.083867</v>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>reserve_fuel [N]</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>4058.128921152442</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5380,6 +5580,14 @@
       <c r="E27" s="2" t="n">
         <v>0.2</v>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Mff</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0.8239224430163152</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -5398,6 +5606,14 @@
       <c r="E28" s="2" t="n">
         <v>0.4</v>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>MTOW [N]</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>2585704.03231381</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -5416,6 +5632,14 @@
       <c r="E29" s="2" t="n">
         <v>0.4</v>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>LD</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>23.95928996628532</v>
+      </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
@@ -5426,6 +5650,14 @@
       <c r="E30" s="2" t="n">
         <v>0.12</v>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>total_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>52407.69572612447</v>
+      </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
@@ -5436,6 +5668,14 @@
       <c r="E31" s="2" t="n">
         <v>0.2</v>
       </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>mission_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>51903.21685673379</v>
+      </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
@@ -5446,6 +5686,14 @@
       <c r="E32" s="2" t="n">
         <v>4.5</v>
       </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>reserve_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>504.4788693906718</v>
+      </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
@@ -5455,6 +5703,14 @@
       </c>
       <c r="E33" s="2" t="n">
         <v>1.5</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>max_fuel_L [L]</t>
+        </is>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>57648.46529873692</v>
       </c>
     </row>
     <row r="34">

</xml_diff>

<commit_message>
added V_cruise to iteration
</commit_message>
<xml_diff>
--- a/concepts.xlsx
+++ b/concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 1 Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 2 Data" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 3 Data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design 4 Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Design 1 Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Design 2 Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Design 3 Data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Design 4 Data" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -435,7 +435,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2617392.438704581</v>
+        <v>2603080.953706842</v>
       </c>
     </row>
     <row r="3">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1285661.953098126</v>
+        <v>1280607.806981</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1285236.953098126</v>
+        <v>1280182.806981</v>
       </c>
     </row>
     <row r="5">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2175348.595536831</v>
+        <v>2170280.137934707</v>
       </c>
     </row>
     <row r="6">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.07818726537040915</v>
+        <v>0.07840172138652085</v>
       </c>
     </row>
     <row r="7">
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.614066979218405</v>
+        <v>1.612647157310132</v>
       </c>
     </row>
     <row r="8">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>13.60287981353899</v>
+        <v>14.14665698449693</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.08479030479090177</v>
+        <v>0.08118727475379874</v>
       </c>
     </row>
     <row r="9">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>30869006.13412389</v>
+        <v>32062671.91010799</v>
       </c>
     </row>
     <row r="12">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01803919235592528</v>
+        <v>0.01667904440331107</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>115.749</v>
+        <v>131.4215948535451</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>54951.87130699764</v>
+        <v>53802.8412734809</v>
       </c>
     </row>
     <row r="14">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>54398.46009909947</v>
+        <v>53271.49035968277</v>
       </c>
     </row>
     <row r="15">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>553.4112078981784</v>
+        <v>531.3509137981353</v>
       </c>
     </row>
     <row r="16">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>60447.05843769741</v>
+        <v>59183.12540082901</v>
       </c>
     </row>
     <row r="17">
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>266808.6074112722</v>
+        <v>265349.7404390257</v>
       </c>
     </row>
     <row r="18">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>131.9519275497795</v>
+        <v>130.7716718421227</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>523.4532863736213</v>
+        <v>520.5935487946512</v>
       </c>
     </row>
     <row r="19">
@@ -1081,7 +1081,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>38.76733331465219</v>
+        <v>38.79710033048644</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>51.15922626338387</v>
+        <v>51.01928796027298</v>
       </c>
     </row>
     <row r="20">
@@ -1123,7 +1123,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>10.23184525267678</v>
+        <v>10.2038575920546</v>
       </c>
     </row>
     <row r="21">
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>24.36767682759289</v>
+        <v>24.25845261531642</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.07960113449328854</v>
+        <v>0.07795204241175259</v>
       </c>
     </row>
     <row r="22">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>7.933580567713551</v>
+        <v>7.898019562281173</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1191,7 +1191,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>1285661.953098126</v>
+        <v>1280607.806981</v>
       </c>
     </row>
     <row r="23">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>2.896498022327736</v>
+        <v>2.883514933415014</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>442043.8431677504</v>
+        <v>432800.8157721351</v>
       </c>
     </row>
     <row r="24">
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>486248.2274845255</v>
+        <v>476080.8973493486</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>437592.0927291759</v>
+        <v>428526.5227513601</v>
       </c>
     </row>
     <row r="26">
@@ -1321,7 +1321,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>4451.750438574527</v>
+        <v>70505.03830755112</v>
       </c>
     </row>
     <row r="27">
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="H27" s="2" t="n">
-        <v>5.805498150852666</v>
+        <v>5.77947593433667</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>0.8116970918239795</v>
+        <v>0.8162038896812348</v>
       </c>
     </row>
     <row r="28">
@@ -1389,7 +1389,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>21.9559591293099</v>
+        <v>22.81335594475067</v>
       </c>
     </row>
     <row r="29">
@@ -1423,7 +1423,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>2617392.438704581</v>
+        <v>2603080.953706842</v>
       </c>
     </row>
     <row r="30">
@@ -1441,7 +1441,7 @@
         </is>
       </c>
       <c r="H30" s="2" t="n">
-        <v>18.51729201240903</v>
+        <v>18.47179541113753</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="K30" s="2" t="n">
-        <v>54951.87130699764</v>
+        <v>53802.8412734809</v>
       </c>
     </row>
     <row r="31">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>68.00178883777365</v>
+        <v>68.03300020382603</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1475,7 +1475,7 @@
         </is>
       </c>
       <c r="K31" s="2" t="n">
-        <v>54398.46009909947</v>
+        <v>53271.49035968277</v>
       </c>
     </row>
     <row r="32">
@@ -1493,7 +1493,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>0.9442534378654445</v>
+        <v>0.944496554819535</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1501,7 +1501,7 @@
         </is>
       </c>
       <c r="K32" s="2" t="n">
-        <v>553.4112078981784</v>
+        <v>8764.704794454528</v>
       </c>
     </row>
     <row r="33">
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="K33" s="2" t="n">
-        <v>60447.05843769741</v>
+        <v>59183.125400829</v>
       </c>
     </row>
     <row r="34">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>62.52721243247608</v>
+        <v>61.94110594244843</v>
       </c>
     </row>
     <row r="36">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>35.91897533095006</v>
+        <v>35.96212349440898</v>
       </c>
     </row>
     <row r="37">
@@ -1605,7 +1605,7 @@
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>9.684566002083631</v>
+        <v>9.639069400812128</v>
       </c>
     </row>
     <row r="39">
@@ -1623,7 +1623,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>9.459246179003902</v>
+        <v>9.414808095599591</v>
       </c>
     </row>
     <row r="40">
@@ -1641,7 +1641,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>3.453508490440939</v>
+        <v>3.437284438816577</v>
       </c>
     </row>
     <row r="41">
@@ -1669,7 +1669,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>14.61692178953825</v>
+        <v>14.57693941722085</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>5.846768715815301</v>
+        <v>5.830775766888342</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1695,7 +1695,7 @@
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>6.921923302090309</v>
+        <v>6.889405171237632</v>
       </c>
     </row>
     <row r="44">
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>10.96269134215369</v>
+        <v>10.93270456291564</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1731,7 +1731,7 @@
         </is>
       </c>
       <c r="H45" s="2" t="n">
-        <v>65.31892490876199</v>
+        <v>65.36336299216629</v>
       </c>
     </row>
     <row r="46">
@@ -1741,7 +1741,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>29.09160917720747</v>
+        <v>29.09417947257073</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1749,7 +1749,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>0.906314874066755</v>
+        <v>0.9067362205573668</v>
       </c>
     </row>
     <row r="47">
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>10.8582847579427</v>
+        <v>10.82858356707835</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>523.4532863736213</v>
+        <v>520.5935487946512</v>
       </c>
     </row>
     <row r="49">
@@ -1787,7 +1787,7 @@
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>51.15922626338387</v>
+        <v>51.01928796027298</v>
       </c>
       <c r="G49" s="1" t="inlineStr">
         <is>
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>32.12548784362076</v>
+        <v>32.11397360404483</v>
       </c>
     </row>
     <row r="51">
@@ -1872,10 +1872,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="23" customWidth="1" min="8" max="8"/>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2503039.137312373</v>
+        <v>2493673.602391189</v>
       </c>
     </row>
     <row r="3">
@@ -1993,7 +1993,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1245277.723627652</v>
+        <v>1241970.255397473</v>
       </c>
     </row>
     <row r="4">
@@ -2029,7 +2029,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1244852.723627652</v>
+        <v>1241545.255397473</v>
       </c>
     </row>
     <row r="5">
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2134850.012764964</v>
+        <v>2131533.178999864</v>
       </c>
     </row>
     <row r="6">
@@ -2099,7 +2099,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.1133586614689065</v>
+        <v>0.1135712517768871</v>
       </c>
     </row>
     <row r="7">
@@ -2133,7 +2133,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.746846312631727</v>
+        <v>1.74609996330969</v>
       </c>
     </row>
     <row r="8">
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.1139206246508157</v>
+        <v>0.1145745109026547</v>
       </c>
     </row>
     <row r="9">
@@ -2266,7 +2266,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>21971782.06303357</v>
+        <v>21764645.40625336</v>
       </c>
     </row>
     <row r="12">
@@ -2284,7 +2284,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.02019118765257179</v>
+        <v>0.01869434128869154</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2304,7 +2304,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>115.749</v>
+        <v>107.8010819767686</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>50347.83284877915</v>
+        <v>49520.70631392276</v>
       </c>
     </row>
     <row r="14">
@@ -2354,7 +2354,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>18.1833321113117</v>
+        <v>18.89728095709556</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>45770.75713525377</v>
+        <v>45018.82392174796</v>
       </c>
     </row>
     <row r="15">
@@ -2396,7 +2396,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>45395.4605126618</v>
+        <v>44658.30838326214</v>
       </c>
     </row>
     <row r="16">
@@ -2430,7 +2430,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>375.2966225919616</v>
+        <v>360.5155384858199</v>
       </c>
     </row>
     <row r="17">
@@ -2456,7 +2456,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>255151.7978911695</v>
+        <v>255819.0902605484</v>
       </c>
     </row>
     <row r="18">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>498.0472605799501</v>
+        <v>499.3594255991807</v>
       </c>
     </row>
     <row r="19">
@@ -2518,7 +2518,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>125.0452910997887</v>
+        <v>125.6100567012792</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>70.57246350949853</v>
+        <v>70.6653681515338</v>
       </c>
     </row>
     <row r="20">
@@ -2552,7 +2552,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>26.84653648783359</v>
+        <v>26.83160257570334</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>7.057246350949852</v>
+        <v>7.06653681515338</v>
       </c>
     </row>
     <row r="21">
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.06642706707267586</v>
+        <v>0.06534839415275384</v>
       </c>
     </row>
     <row r="22">
@@ -2620,7 +2620,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>23.72137875312161</v>
+        <v>23.77488706925348</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2628,7 +2628,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>1245277.723627652</v>
+        <v>1247589.512983257</v>
       </c>
     </row>
     <row r="23">
@@ -2646,7 +2646,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>7.723160104537921</v>
+        <v>7.740581237462429</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2654,7 +2654,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>368189.1245474084</v>
+        <v>372416.9271972666</v>
       </c>
     </row>
     <row r="24">
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>6.141306450810832</v>
+        <v>6.15124490581902</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2690,7 +2690,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>405008.0370021492</v>
+        <v>409658.6199169933</v>
       </c>
     </row>
     <row r="25">
@@ -2724,7 +2724,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>365170.1634559541</v>
+        <v>359240.3642966373</v>
       </c>
     </row>
     <row r="26">
@@ -2750,7 +2750,7 @@
         </is>
       </c>
       <c r="H26" s="2" t="n">
-        <v>0.7951805177782558</v>
+        <v>0.7946748076292477</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2758,7 +2758,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>3018.961091454257</v>
+        <v>68628.01953390805</v>
       </c>
     </row>
     <row r="27">
@@ -2784,7 +2784,7 @@
         </is>
       </c>
       <c r="H27" s="2" t="n">
-        <v>6.962313302412682</v>
+        <v>6.97621854227058</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>0.8529031691678821</v>
+        <v>0.8516022026270456</v>
       </c>
     </row>
     <row r="28">
@@ -2826,7 +2826,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>2503039.137312373</v>
+        <v>2509585.27545598</v>
       </c>
     </row>
     <row r="29">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>31.76340890548123</v>
+        <v>33.01344764824431</v>
       </c>
     </row>
     <row r="30">
@@ -2878,7 +2878,7 @@
         </is>
       </c>
       <c r="H30" s="2" t="n">
-        <v>15.7976164097961</v>
+        <v>15.82094491354527</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2886,7 +2886,7 @@
         </is>
       </c>
       <c r="K30" s="2" t="n">
-        <v>45770.75713525377</v>
+        <v>46296.32868368099</v>
       </c>
     </row>
     <row r="31">
@@ -2904,7 +2904,7 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>45.25618737474902</v>
+        <v>45.23992681082278</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="K31" s="2" t="n">
-        <v>45395.4605126618</v>
+        <v>44658.30838326214</v>
       </c>
     </row>
     <row r="32">
@@ -2930,7 +2930,7 @@
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>0.9213410529202575</v>
+        <v>0.9211635972781035</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2938,7 +2938,7 @@
         </is>
       </c>
       <c r="K32" s="2" t="n">
-        <v>375.2966225919616</v>
+        <v>8531.366641046723</v>
       </c>
     </row>
     <row r="33">
@@ -2956,7 +2956,7 @@
         </is>
       </c>
       <c r="K33" s="2" t="n">
-        <v>50347.83284877915</v>
+        <v>50925.96155204909</v>
       </c>
     </row>
     <row r="34">
@@ -2994,7 +2994,7 @@
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>61.34802317489211</v>
+        <v>61.64676724338313</v>
       </c>
     </row>
     <row r="36">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>24.02516467246105</v>
+        <v>24.00336099178257</v>
       </c>
     </row>
     <row r="37">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>9.592811619245849</v>
+        <v>9.616140122995022</v>
       </c>
     </row>
     <row r="39">
@@ -3060,7 +3060,7 @@
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>9.369626541419894</v>
+        <v>9.392412287307085</v>
       </c>
     </row>
     <row r="40">
@@ -3078,7 +3078,7 @@
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>3.420788950907906</v>
+        <v>3.429107876686274</v>
       </c>
     </row>
     <row r="41">
@@ -3106,7 +3106,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>10.08178050135693</v>
+        <v>10.09506323599489</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -3124,7 +3124,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>4.032712200542774</v>
+        <v>4.038025294397958</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>6.856342996220422</v>
+        <v>6.873016754618014</v>
       </c>
     </row>
     <row r="44">
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>15.1226707520354</v>
+        <v>15.14259485399234</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -3160,7 +3160,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>19.99790229800873</v>
+        <v>19.99645511244436</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -3168,7 +3168,7 @@
         </is>
       </c>
       <c r="H45" s="2" t="n">
-        <v>43.07121417825724</v>
+        <v>43.04842843237005</v>
       </c>
     </row>
     <row r="46">
@@ -3178,7 +3178,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>19.34978783720721</v>
+        <v>19.34748676155897</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -3186,7 +3186,7 @@
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>0.8678460426622649</v>
+        <v>0.8675384939257296</v>
       </c>
     </row>
     <row r="47">
@@ -3196,7 +3196,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>7.489322658150864</v>
+        <v>7.49918983245335</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -3214,7 +3214,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>498.0472605799501</v>
+        <v>499.360478519805</v>
       </c>
     </row>
     <row r="49">
@@ -3224,7 +3224,7 @@
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>70.57246350949853</v>
+        <v>70.66544265196427</v>
       </c>
       <c r="G49" s="1" t="inlineStr">
         <is>
@@ -3252,7 +3252,7 @@
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>21.74576523265384</v>
+        <v>21.75132832310466</v>
       </c>
     </row>
     <row r="51">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>DESIGN_OEW_FUEL</t>
+          <t>ALTITUDE_OEW_FUEL</t>
         </is>
       </c>
     </row>
@@ -3274,7 +3274,7 @@
         </is>
       </c>
       <c r="H52" s="2" t="n">
-        <v>20.35857755988187</v>
+        <v>20.37148878167033</v>
       </c>
     </row>
     <row r="53">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>ALTITUDE_OEW_PAYLOAD</t>
+          <t>DESIGN_OEW_PAYLOAD</t>
         </is>
       </c>
     </row>
@@ -3309,10 +3309,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
@@ -3394,7 +3394,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2538643.19660158</v>
+        <v>2528141.247637751</v>
       </c>
     </row>
     <row r="3">
@@ -3430,7 +3430,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1257851.409589583</v>
+        <v>1254142.613151885</v>
       </c>
     </row>
     <row r="4">
@@ -3466,7 +3466,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1257426.409589583</v>
+        <v>1253717.613151885</v>
       </c>
     </row>
     <row r="5">
@@ -3502,7 +3502,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2147459.302786185</v>
+        <v>2143740.004399523</v>
       </c>
     </row>
     <row r="6">
@@ -3536,7 +3536,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.15686224662124</v>
+        <v>0.1571875370108455</v>
       </c>
     </row>
     <row r="7">
@@ -3570,7 +3570,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.65595971619502</v>
+        <v>1.655019454406412</v>
       </c>
     </row>
     <row r="8">
@@ -3604,7 +3604,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.1056343876060222</v>
+        <v>0.1063090202835842</v>
       </c>
     </row>
     <row r="9">
@@ -3703,7 +3703,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>24032355.88461775</v>
+        <v>23781060.54306415</v>
       </c>
     </row>
     <row r="12">
@@ -3721,7 +3721,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01893559574219003</v>
+        <v>0.01756352718180103</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3741,7 +3741,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>115.749</v>
+        <v>115.2476898121415</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>53492.24076936609</v>
+        <v>52564.75069765191</v>
       </c>
     </row>
     <row r="14">
@@ -3791,7 +3791,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.79422279929057</v>
+        <v>17.43787372561123</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -3799,7 +3799,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>48629.30979033281</v>
+        <v>47786.13699786537</v>
       </c>
     </row>
     <row r="15">
@@ -3833,7 +3833,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>48198.09536232964</v>
+        <v>47371.37173563943</v>
       </c>
     </row>
     <row r="16">
@@ -3867,7 +3867,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>431.2144280031645</v>
+        <v>414.7652622259322</v>
       </c>
     </row>
     <row r="17">
@@ -3893,7 +3893,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>258781.1617330866</v>
+        <v>257710.6266705149</v>
       </c>
     </row>
     <row r="18">
@@ -3929,7 +3929,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>508.0110411992717</v>
+        <v>505.9106186859496</v>
       </c>
     </row>
     <row r="19">
@@ -3955,7 +3955,7 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>100.4155389133867</v>
+        <v>99.74020283736353</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -3963,7 +3963,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>63.75020258473045</v>
+        <v>63.61827527910197</v>
       </c>
     </row>
     <row r="20">
@@ -3989,7 +3989,7 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>38.50468574757637</v>
+        <v>38.52522865219755</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -3997,7 +3997,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>7.968775323091307</v>
+        <v>7.952284409887746</v>
       </c>
     </row>
     <row r="21">
@@ -4023,7 +4023,7 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>21.25723230127196</v>
+        <v>21.18562986479599</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -4031,7 +4031,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.07052815583874701</v>
+        <v>0.06931841316446796</v>
       </c>
     </row>
     <row r="22">
@@ -4057,7 +4057,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>6.920888121668483</v>
+        <v>6.897575940427495</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -4065,7 +4065,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>1257851.409589583</v>
+        <v>1254142.613151885</v>
       </c>
     </row>
     <row r="23">
@@ -4083,7 +4083,7 @@
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>2.526770678896832</v>
+        <v>2.51825955503739</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -4091,7 +4091,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>391183.8938153951</v>
+        <v>384401.2432382285</v>
       </c>
     </row>
     <row r="24">
@@ -4127,7 +4127,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>430302.2831969347</v>
+        <v>422841.3675620515</v>
       </c>
     </row>
     <row r="25">
@@ -4161,7 +4161,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>387715.1187136521</v>
+        <v>381064.7885158307</v>
       </c>
     </row>
     <row r="26">
@@ -4187,7 +4187,7 @@
         </is>
       </c>
       <c r="H26" s="2" t="n">
-        <v>5.064447616013075</v>
+        <v>5.047388631871958</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -4195,7 +4195,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>3468.775101743056</v>
+        <v>69170.5770837997</v>
       </c>
     </row>
     <row r="27">
@@ -4229,7 +4229,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>0.8437236981652552</v>
+        <v>0.8470434661266297</v>
       </c>
     </row>
     <row r="28">
@@ -4263,7 +4263,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>2538643.19660158</v>
+        <v>2528141.247637751</v>
       </c>
     </row>
     <row r="29">
@@ -4297,7 +4297,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>27.81055642042914</v>
+        <v>28.86256860717857</v>
       </c>
     </row>
     <row r="30">
@@ -4315,7 +4315,7 @@
         </is>
       </c>
       <c r="H30" s="2" t="n">
-        <v>67.8572829660974</v>
+        <v>67.88059514733837</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -4323,7 +4323,7 @@
         </is>
       </c>
       <c r="K30" s="2" t="n">
-        <v>48629.30979033281</v>
+        <v>47786.13699786537</v>
       </c>
     </row>
     <row r="31">
@@ -4341,7 +4341,7 @@
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>0.9374134265694098</v>
+        <v>0.9376107824411253</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -4349,7 +4349,7 @@
         </is>
       </c>
       <c r="K31" s="2" t="n">
-        <v>48198.09536232964</v>
+        <v>47371.37173563943</v>
       </c>
     </row>
     <row r="32">
@@ -4367,7 +4367,7 @@
         </is>
       </c>
       <c r="K32" s="2" t="n">
-        <v>431.2144280031645</v>
+        <v>8598.813689838604</v>
       </c>
     </row>
     <row r="33">
@@ -4395,7 +4395,7 @@
         </is>
       </c>
       <c r="K33" s="2" t="n">
-        <v>53492.24076936609</v>
+        <v>52564.75069765191</v>
       </c>
     </row>
     <row r="34">
@@ -4413,7 +4413,7 @@
         </is>
       </c>
       <c r="H34" s="2" t="n">
-        <v>76.61861886040808</v>
+        <v>76.07477242254149</v>
       </c>
     </row>
     <row r="35">
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>35.44961392675044</v>
+        <v>35.48183993391456</v>
       </c>
     </row>
     <row r="36">
@@ -4441,7 +4441,7 @@
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>10.72044440732809</v>
+        <v>10.68232927005212</v>
       </c>
     </row>
     <row r="37">
@@ -4461,7 +4461,7 @@
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>10.4710239752018</v>
+        <v>10.43379561963457</v>
       </c>
     </row>
     <row r="38">
@@ -4479,7 +4479,7 @@
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>3.822901901235648</v>
+        <v>3.809310073768257</v>
       </c>
     </row>
     <row r="39">
@@ -4543,7 +4543,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>11.3839647472733</v>
+        <v>11.36040629983964</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4551,7 +4551,7 @@
         </is>
       </c>
       <c r="H42" s="2" t="n">
-        <v>64.30714711256408</v>
+        <v>64.34437546813132</v>
       </c>
     </row>
     <row r="43">
@@ -4561,7 +4561,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>4.553585898909319</v>
+        <v>4.544162519935855</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4569,7 +4569,7 @@
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>0.8967215480038735</v>
+        <v>0.8970745343562955</v>
       </c>
     </row>
     <row r="44">
@@ -4579,7 +4579,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>13.66075769672796</v>
+        <v>13.63248755980757</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>7.66230453030963</v>
+        <v>7.635062209196207</v>
       </c>
     </row>
     <row r="45">
@@ -4615,7 +4615,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>29.2994421299245</v>
+        <v>29.30095660154523</v>
       </c>
     </row>
     <row r="47">
@@ -4625,7 +4625,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>8.456659526545877</v>
+        <v>8.43915896559516</v>
       </c>
       <c r="G47" s="1" t="inlineStr">
         <is>
@@ -4645,7 +4645,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>508.0110411992717</v>
+        <v>505.9106186859496</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
         </is>
       </c>
       <c r="H48" s="2" t="n">
-        <v>31.87459987237063</v>
+        <v>31.86887394459232</v>
       </c>
     </row>
     <row r="49">
@@ -4663,7 +4663,7 @@
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>63.75020258473045</v>
+        <v>63.61827527910197</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -4726,10 +4726,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
@@ -4811,7 +4811,7 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2585704.03231381</v>
+        <v>2572803.758039543</v>
       </c>
     </row>
     <row r="3">
@@ -4847,7 +4847,7 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>1274471.092321406</v>
+        <v>1269915.319727336</v>
       </c>
     </row>
     <row r="4">
@@ -4883,7 +4883,7 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>1274046.092321406</v>
+        <v>1269490.319727336</v>
       </c>
     </row>
     <row r="5">
@@ -4919,7 +4919,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>2164126.04635372</v>
+        <v>2159557.373485375</v>
       </c>
     </row>
     <row r="6">
@@ -4953,7 +4953,7 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.09749748833112409</v>
+        <v>0.09774161916751845</v>
       </c>
     </row>
     <row r="7">
@@ -4987,7 +4987,7 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.489981645027543</v>
+        <v>1.488959492951389</v>
       </c>
     </row>
     <row r="8">
@@ -5021,7 +5021,7 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.09357096497711698</v>
+        <v>0.094312379495055</v>
       </c>
     </row>
     <row r="9">
@@ -5120,7 +5120,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>27633615.11710551</v>
+        <v>27279597.56517904</v>
       </c>
     </row>
     <row r="12">
@@ -5138,7 +5138,7 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.01470646584450298</v>
+        <v>0.01360300344108735</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -5158,7 +5158,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>115.749</v>
+        <v>128.4722557060539</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>57648.46529873692</v>
+        <v>56509.16474100405</v>
       </c>
     </row>
     <row r="14">
@@ -5208,7 +5208,7 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.08025846911854</v>
+        <v>16.71975004337757</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -5216,7 +5216,7 @@
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>52407.69572612447</v>
+        <v>51371.96794636732</v>
       </c>
     </row>
     <row r="15">
@@ -5250,7 +5250,7 @@
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>51903.21685673379</v>
+        <v>50887.50059323582</v>
       </c>
     </row>
     <row r="16">
@@ -5276,7 +5276,7 @@
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>504.4788693906718</v>
+        <v>484.4673531315003</v>
       </c>
     </row>
     <row r="17">
@@ -5312,7 +5312,7 @@
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>263578.3926925393</v>
+        <v>262263.3800244183</v>
       </c>
     </row>
     <row r="18">
@@ -5338,7 +5338,7 @@
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>561.0633135905323</v>
+        <v>558.2640598537121</v>
       </c>
     </row>
     <row r="19">
@@ -5374,7 +5374,7 @@
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>41.02669790236105</v>
+        <v>40.92422484985068</v>
       </c>
     </row>
     <row r="20">
@@ -5400,7 +5400,7 @@
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>13.67556596745369</v>
+        <v>13.64140828328356</v>
       </c>
     </row>
     <row r="21">
@@ -5436,7 +5436,7 @@
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.07594985111932576</v>
+        <v>0.07446355597879362</v>
       </c>
     </row>
     <row r="22">
@@ -5462,7 +5462,7 @@
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>32.22366166980459</v>
+        <v>32.21111934595463</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -5470,7 +5470,7 @@
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>1274471.092321406</v>
+        <v>1269915.319727336</v>
       </c>
     </row>
     <row r="23">
@@ -5498,7 +5498,7 @@
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>421577.9859600904</v>
+        <v>413246.384554168</v>
       </c>
     </row>
     <row r="24">
@@ -5534,7 +5534,7 @@
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>463735.7845560995</v>
+        <v>454571.0230095848</v>
       </c>
     </row>
     <row r="25">
@@ -5570,7 +5570,7 @@
         </is>
       </c>
       <c r="K25" s="2" t="n">
-        <v>417519.857038938</v>
+        <v>409349.2322721076</v>
       </c>
     </row>
     <row r="26">
@@ -5596,7 +5596,7 @@
         </is>
       </c>
       <c r="K26" s="2" t="n">
-        <v>4058.128921152442</v>
+        <v>69897.80280729913</v>
       </c>
     </row>
     <row r="27">
@@ -5622,7 +5622,7 @@
         </is>
       </c>
       <c r="K27" s="2" t="n">
-        <v>0.8239224430163152</v>
+        <v>0.828084577368043</v>
       </c>
     </row>
     <row r="28">
@@ -5648,7 +5648,7 @@
         </is>
       </c>
       <c r="K28" s="2" t="n">
-        <v>2585704.03231381</v>
+        <v>2572803.758039543</v>
       </c>
     </row>
     <row r="29">
@@ -5674,7 +5674,7 @@
         </is>
       </c>
       <c r="K29" s="2" t="n">
-        <v>23.95928996628532</v>
+        <v>24.89541097931098</v>
       </c>
     </row>
     <row r="30">
@@ -5692,7 +5692,7 @@
         </is>
       </c>
       <c r="K30" s="2" t="n">
-        <v>52407.69572612447</v>
+        <v>51371.96794636732</v>
       </c>
     </row>
     <row r="31">
@@ -5710,7 +5710,7 @@
         </is>
       </c>
       <c r="K31" s="2" t="n">
-        <v>51903.21685673379</v>
+        <v>50887.50059323582</v>
       </c>
     </row>
     <row r="32">
@@ -5728,7 +5728,7 @@
         </is>
       </c>
       <c r="K32" s="2" t="n">
-        <v>504.4788693906718</v>
+        <v>8689.217424641249</v>
       </c>
     </row>
     <row r="33">
@@ -5746,7 +5746,7 @@
         </is>
       </c>
       <c r="K33" s="2" t="n">
-        <v>57648.46529873692</v>
+        <v>56509.16474100405</v>
       </c>
     </row>
     <row r="34">
@@ -5829,7 +5829,7 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>19.53652281064812</v>
+        <v>19.48772611897652</v>
       </c>
     </row>
     <row r="43">
@@ -5839,7 +5839,7 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>7.814609124259249</v>
+        <v>7.795090447590609</v>
       </c>
     </row>
     <row r="44">
@@ -5849,7 +5849,7 @@
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>8.791435264791655</v>
+        <v>8.769476753539433</v>
       </c>
     </row>
     <row r="45">
@@ -5859,7 +5859,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>28.87024079378784</v>
+        <v>28.87314071146432</v>
       </c>
     </row>
     <row r="46">
@@ -5869,7 +5869,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>28.24228113201701</v>
+        <v>28.24674951478293</v>
       </c>
     </row>
     <row r="47">
@@ -5879,7 +5879,7 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>14.51284551648146</v>
+        <v>14.47659654552542</v>
       </c>
     </row>
     <row r="48">
@@ -5889,7 +5889,7 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>561.0633135905323</v>
+        <v>558.2640598537121</v>
       </c>
     </row>
     <row r="49">
@@ -5899,7 +5899,7 @@
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>41.02669790236105</v>
+        <v>40.92422484985068</v>
       </c>
     </row>
     <row r="50">

</xml_diff>